<commit_message>
changed markers based on thresholds review
</commit_message>
<xml_diff>
--- a/bioSample/bioSample_1874.xlsx
+++ b/bioSample/bioSample_1874.xlsx
@@ -142,7 +142,7 @@
     <t xml:space="preserve">CNAG_07528</t>
   </si>
   <si>
-    <t xml:space="preserve">TDY1948</t>
+    <t xml:space="preserve">TDY1970</t>
   </si>
   <si>
     <t xml:space="preserve">CNAG_03115</t>
@@ -160,6 +160,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -244,7 +245,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E43" activeCellId="0" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1590,7 +1591,7 @@
         <v>1</v>
       </c>
       <c r="J41" s="0" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1622,7 +1623,7 @@
         <v>2</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1654,7 +1655,7 @@
         <v>3</v>
       </c>
       <c r="J43" s="0" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>